<commit_message>
generic commit message, Mon 15:29:32 14.08.2023.
</commit_message>
<xml_diff>
--- a/datasets-creation-documentation.xlsx
+++ b/datasets-creation-documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\imageProcessTif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A9FDBC-67F7-4876-A47B-537FD9F0A783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70E1D09-F45B-4322-ADE5-533A98F21ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>dataset</t>
   </si>
@@ -90,9 +90,6 @@
     <t>location after scaling</t>
   </si>
   <si>
-    <t>M:\data\d.walther\Microscopy\babb03\tiff-ct3\dataset03\raw-cropNorm\</t>
-  </si>
-  <si>
     <t>scaling factor</t>
   </si>
   <si>
@@ -108,7 +105,43 @@
     <t>0.085</t>
   </si>
   <si>
-    <t>M:\data\d.walther\Microscopy\babb03\tiff-ct3\dataset03\raw-cropNorm-bicubic-scaled0.25\</t>
+    <t>...\dataset03\raw-cropNorm\</t>
+  </si>
+  <si>
+    <t>...\dataset03\raw-cropNorm-bicubic-scaled0.25\</t>
+  </si>
+  <si>
+    <t>blurring sigma x</t>
+  </si>
+  <si>
+    <t>blurring sigma y</t>
+  </si>
+  <si>
+    <t>blurring sigma z</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>blurring method</t>
+  </si>
+  <si>
+    <t>blur3D</t>
+  </si>
+  <si>
+    <t>threshold label method</t>
+  </si>
+  <si>
+    <t>Otsu</t>
+  </si>
+  <si>
+    <t>threshold value (lower)</t>
+  </si>
+  <si>
+    <t>label filtering/selection</t>
+  </si>
+  <si>
+    <t>Keep Largest Label</t>
   </si>
 </sst>
 </file>
@@ -426,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,13 +474,17 @@
     <col min="6" max="6" width="66.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="62.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="79" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="79" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,19 +510,40 @@
         <v>17</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" t="s">
         <v>19</v>
       </c>
       <c r="K1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L1" t="s">
         <v>20</v>
       </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -502,13 +560,34 @@
         <v>18</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -528,13 +607,34 @@
         <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K3">
         <v>0.25</v>
       </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3">
+        <v>570</v>
+      </c>
+      <c r="S3" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -554,16 +654,37 @@
         <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="K4">
         <v>0.25</v>
       </c>
       <c r="L4" t="s">
         <v>27</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4">
+        <v>570</v>
+      </c>
+      <c r="S4" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>